<commit_message>
added column for used connections/signals in IMU
</commit_message>
<xml_diff>
--- a/Electrical/Pi_ExternalConnections.xlsx
+++ b/Electrical/Pi_ExternalConnections.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub_Local\2018\Electrical\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chedd\Desktop\IEEEHardware\2018\Electrical\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="9874" yWindow="0" windowWidth="18523" windowHeight="10423" xr2:uid="{275B7CE7-B5D7-42A8-8D01-8AF01286FEB7}"/>
+    <workbookView xWindow="9876" yWindow="0" windowWidth="18528" windowHeight="10428" xr2:uid="{275B7CE7-B5D7-42A8-8D01-8AF01286FEB7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="71">
   <si>
     <t>Interface Type</t>
   </si>
@@ -86,9 +86,6 @@
     <t>https://www.sparkfun.com/products/13284</t>
   </si>
   <si>
-    <t>VDD</t>
-  </si>
-  <si>
     <t>ground</t>
   </si>
   <si>
@@ -213,16 +210,51 @@
   </si>
   <si>
     <t>Pin Breakout Interface</t>
+  </si>
+  <si>
+    <t>Which connectors/signals</t>
+  </si>
+  <si>
+    <t>:)</t>
+  </si>
+  <si>
+    <t>VDD/VCC</t>
+  </si>
+  <si>
+    <t>:) connect to 13</t>
+  </si>
+  <si>
+    <t>:) connect to 11</t>
+  </si>
+  <si>
+    <t>:) connect to 12</t>
+  </si>
+  <si>
+    <t>:) connect to 9</t>
+  </si>
+  <si>
+    <t>:) connect to 10</t>
+  </si>
+  <si>
+    <t>bridge to SDOM</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -294,10 +326,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -311,12 +344,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -629,35 +664,36 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91353DA0-C921-4B81-83D7-9273390D1805}">
-  <dimension ref="A1:G24"/>
+  <dimension ref="A1:H24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" topLeftCell="D3" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.23046875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.84375" customWidth="1"/>
-    <col min="3" max="3" width="20.07421875" customWidth="1"/>
-    <col min="4" max="4" width="19.23046875" customWidth="1"/>
-    <col min="5" max="5" width="10.921875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="40.69140625" customWidth="1"/>
-    <col min="7" max="7" width="17.3046875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.88671875" customWidth="1"/>
+    <col min="3" max="3" width="20.109375" customWidth="1"/>
+    <col min="4" max="4" width="19.21875" customWidth="1"/>
+    <col min="5" max="5" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="41.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D1" t="s">
         <v>47</v>
-      </c>
-      <c r="C1" t="s">
-        <v>54</v>
-      </c>
-      <c r="D1" t="s">
-        <v>48</v>
       </c>
       <c r="E1" t="s">
         <v>1</v>
@@ -666,53 +702,56 @@
         <v>12</v>
       </c>
       <c r="G1" t="s">
+        <v>62</v>
+      </c>
+      <c r="H1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" s="2" customFormat="1" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A2" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="C2" s="2" t="s">
+      <c r="F2" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" s="6" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="5"/>
+      <c r="B3" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="F2" s="2" t="s">
+      <c r="D3" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="F3" s="6" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="3" spans="1:7" s="6" customFormat="1" ht="44.15" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A3" s="5"/>
-      <c r="B3" s="10" t="s">
-        <v>58</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="F3" s="6" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>3</v>
@@ -721,7 +760,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:7" s="6" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:8" s="6" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="5"/>
       <c r="E5" s="6" t="s">
         <v>4</v>
@@ -730,37 +769,37 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C6" s="8"/>
-      <c r="D6" s="9" t="s">
-        <v>49</v>
+      <c r="D6" s="10" t="s">
+        <v>48</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>6</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="G6" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H6" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3"/>
       <c r="E7" s="4" t="s">
         <v>7</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.4">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3"/>
       <c r="E8" s="4" t="s">
         <v>8</v>
@@ -769,7 +808,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3"/>
       <c r="E9" s="4" t="s">
         <v>13</v>
@@ -778,7 +817,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:7" s="6" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:8" s="6" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="5"/>
       <c r="E10" s="6" t="s">
         <v>14</v>
@@ -787,126 +826,154 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>18</v>
       </c>
-      <c r="G11" t="s">
+      <c r="H11" s="11" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E12" t="s">
         <v>7</v>
       </c>
       <c r="F12" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.4">
+        <v>20</v>
+      </c>
+      <c r="G12" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="E13" t="s">
-        <v>20</v>
+        <v>64</v>
       </c>
       <c r="F13" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.4">
+        <v>22</v>
+      </c>
+      <c r="G13" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="E14" t="s">
         <v>14</v>
       </c>
       <c r="F14" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.4">
+        <v>23</v>
+      </c>
+      <c r="G14" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="E15" t="s">
         <v>13</v>
       </c>
       <c r="F15" t="s">
+        <v>24</v>
+      </c>
+      <c r="G15" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A16" t="s">
-        <v>26</v>
-      </c>
       <c r="E16" t="s">
+        <v>27</v>
+      </c>
+      <c r="F16" t="s">
         <v>28</v>
       </c>
-      <c r="F16" t="s">
+    </row>
+    <row r="17" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E17" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="17" spans="5:6" x14ac:dyDescent="0.4">
-      <c r="E17" t="s">
+      <c r="F17" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="18" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E18" t="s">
         <v>30</v>
       </c>
-      <c r="F17" t="s">
+      <c r="F18" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="18" spans="5:6" x14ac:dyDescent="0.4">
-      <c r="E18" t="s">
+    <row r="19" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E19" t="s">
         <v>31</v>
       </c>
-      <c r="F18" t="s">
+      <c r="F19" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="20" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E20" t="s">
+        <v>33</v>
+      </c>
+      <c r="F20" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="21" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E21" t="s">
+        <v>35</v>
+      </c>
+      <c r="F21" t="s">
+        <v>36</v>
+      </c>
+      <c r="G21" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="22" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E22" t="s">
+        <v>37</v>
+      </c>
+      <c r="F22" t="s">
+        <v>38</v>
+      </c>
+      <c r="G22" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="23" spans="5:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="E23" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="19" spans="5:6" x14ac:dyDescent="0.4">
-      <c r="E19" t="s">
-        <v>32</v>
-      </c>
-      <c r="F19" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="20" spans="5:6" x14ac:dyDescent="0.4">
-      <c r="E20" t="s">
-        <v>34</v>
-      </c>
-      <c r="F20" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="21" spans="5:6" x14ac:dyDescent="0.4">
-      <c r="E21" t="s">
-        <v>36</v>
-      </c>
-      <c r="F21" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="22" spans="5:6" x14ac:dyDescent="0.4">
-      <c r="E22" t="s">
-        <v>38</v>
-      </c>
-      <c r="F22" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="23" spans="5:6" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="E23" t="s">
+      <c r="F23" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="G23" s="7" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="24" spans="5:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="E24" t="s">
         <v>42</v>
       </c>
-      <c r="F23" s="7" t="s">
+      <c r="F24" s="7" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="24" spans="5:6" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="E24" t="s">
-        <v>43</v>
-      </c>
-      <c r="F24" s="7" t="s">
-        <v>45</v>
+      <c r="G24" s="7" t="s">
+        <v>70</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D6" r:id="rId1" xr:uid="{E6746FDF-F36C-4A2B-8D7F-300AA30307B3}"/>
+    <hyperlink ref="H11" r:id="rId2" xr:uid="{5F21002E-9BEF-4D8B-A196-D38A72CF76FC}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
finished footprints on Pi cape. onto layouts
</commit_message>
<xml_diff>
--- a/Electrical/Pi_ExternalConnections.xlsx
+++ b/Electrical/Pi_ExternalConnections.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="42">
   <si>
     <t xml:space="preserve">Interface</t>
   </si>
@@ -40,9 +40,6 @@
     <t xml:space="preserve">Signal Description</t>
   </si>
   <si>
-    <t xml:space="preserve">Signals Used</t>
-  </si>
-  <si>
     <t xml:space="preserve">Connector</t>
   </si>
   <si>
@@ -58,9 +55,6 @@
     <t xml:space="preserve">Interface to Pi &amp;Breakout</t>
   </si>
   <si>
-    <t xml:space="preserve">n/a</t>
-  </si>
-  <si>
     <t xml:space="preserve">40-pins (2 rows of 20) extra long female headers</t>
   </si>
   <si>
@@ -73,76 +67,85 @@
     <t xml:space="preserve">power</t>
   </si>
   <si>
+    <t xml:space="preserve">3-pin female latched 0.1" header</t>
+  </si>
+  <si>
+    <t xml:space="preserve">digikey</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.digikey.com/products/en?keywords=WM4825-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ground from arduino</t>
+  </si>
+  <si>
+    <t xml:space="preserve">serial</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pi's transmit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pi's receive</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Distance Sensor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">input voltage (use 3.3V for our logic levels)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5-pin snapping connector</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.digikey.com/products/en?keywords=WM4827-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ground</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SHDN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shutdown(pull low to shutdown)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SCL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">i2c serial clock</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SDA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">i2c serial data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5V Power from Voltage Regulator</t>
+  </si>
+  <si>
     <t xml:space="preserve">PWR_5V</t>
   </si>
   <si>
     <t xml:space="preserve">5V power from arduino</t>
   </si>
   <si>
-    <t xml:space="preserve">all</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4-pin female latched 0.1" header</t>
-  </si>
-  <si>
-    <t xml:space="preserve">digikey</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GND</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ground from arduino</t>
-  </si>
-  <si>
-    <t xml:space="preserve">serial</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tx</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pi's transmit</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rx</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pi's receive</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Distance Sensor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vin</t>
-  </si>
-  <si>
-    <t xml:space="preserve">input voltage (use 3.3V for our logic levels)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5-pin snapping connector</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.digikey.com/products/en?keywords=WM4827-ND</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ground</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SHDN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Shutdown(pull low to shutdown)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SCL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">i2c serial clock</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SDA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">i2c serial data</t>
+    <t xml:space="preserve">2-pin female latched 0.1" header</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.digikey.com/products/en?keywords=WM4824-ND</t>
   </si>
 </sst>
 </file>
@@ -200,7 +203,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="14">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -282,6 +285,20 @@
       <left/>
       <right/>
       <top style="thin"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin"/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right style="thin"/>
+      <top/>
       <bottom/>
       <diagonal/>
     </border>
@@ -314,7 +331,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="36">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -435,15 +452,27 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="10" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -525,31 +554,30 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J12"/>
+  <dimension ref="1:13"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="D1" activeCellId="0" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J8" activeCellId="0" sqref="J8"/>
+      <selection pane="bottomRight" activeCell="I4" activeCellId="0" sqref="I4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="20.4615384615385"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="20.5668016194332"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="2" width="9"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="3" width="6.31983805668016"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="2" width="7.60728744939271"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.1052631578947"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="39.9554655870445"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="19.8178137651822"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="48.7408906882591"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="4" width="7.39271255060729"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.57085020242915"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.2105263157895"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="40.2753036437247"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="49.165991902834"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="4" width="7.49797570850202"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
-    <row r="1" s="9" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" s="9" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -568,209 +596,238 @@
       <c r="F1" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="G1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="AMJ1" s="0"/>
+    </row>
+    <row r="2" s="15" customFormat="true" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="10" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" s="15" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="11" t="s">
+      <c r="B2" s="12" t="s">
         <v>8</v>
-      </c>
-      <c r="B2" s="12" t="s">
-        <v>9</v>
       </c>
       <c r="C2" s="13" t="n">
         <v>1</v>
       </c>
       <c r="D2" s="14"/>
       <c r="E2" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="15" t="s">
+      <c r="G2" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="15" t="s">
+      <c r="H2" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="H2" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="I2" s="17" t="s">
-        <v>14</v>
-      </c>
+      <c r="AMJ2" s="0"/>
     </row>
     <row r="3" customFormat="false" ht="14.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="11" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B3" s="12"/>
       <c r="C3" s="13"/>
       <c r="D3" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="15"/>
+      <c r="F3" s="15"/>
+      <c r="G3" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="H3" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="15" t="s">
+      <c r="I3" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="F3" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="G3" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="H3" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="I3" s="19" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="4" s="2" customFormat="true" ht="14.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="4" s="2" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1"/>
       <c r="C4" s="3"/>
       <c r="D4" s="18"/>
       <c r="E4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G4" s="20"/>
+      <c r="H4" s="21"/>
+      <c r="AMJ4" s="0"/>
+    </row>
+    <row r="5" customFormat="false" ht="14.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0"/>
+      <c r="B5" s="0"/>
+      <c r="C5" s="0"/>
+      <c r="D5" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F5" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F4" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="H4" s="20"/>
-      <c r="I4" s="21"/>
-    </row>
-    <row r="5" customFormat="false" ht="14.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D5" s="22" t="s">
-        <v>24</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="G5" s="2"/>
-      <c r="I5" s="21"/>
-    </row>
-    <row r="6" s="24" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G5" s="0"/>
+      <c r="H5" s="21"/>
+    </row>
+    <row r="6" s="24" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="23"/>
       <c r="C6" s="25"/>
       <c r="D6" s="22"/>
       <c r="E6" s="24" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="F6" s="24" t="s">
-        <v>28</v>
-      </c>
-      <c r="H6" s="23"/>
-      <c r="I6" s="26"/>
+        <v>24</v>
+      </c>
+      <c r="G6" s="23"/>
+      <c r="H6" s="26"/>
+      <c r="AMJ6" s="0"/>
     </row>
     <row r="7" s="15" customFormat="true" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="11" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C7" s="13" t="n">
         <v>8</v>
       </c>
       <c r="D7" s="27"/>
       <c r="E7" s="15" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="F7" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="G7" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="H7" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="I7" s="21" t="s">
-        <v>21</v>
-      </c>
-      <c r="J7" s="15" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="8" s="2" customFormat="true" ht="14.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>27</v>
+      </c>
+      <c r="G7" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="H7" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="I7" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="AMJ7" s="0"/>
+    </row>
+    <row r="8" s="2" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1"/>
       <c r="C8" s="3"/>
       <c r="D8" s="27"/>
       <c r="E8" s="2" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="H8" s="1"/>
-      <c r="I8" s="4"/>
-    </row>
-    <row r="9" s="2" customFormat="true" ht="14.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>30</v>
+      </c>
+      <c r="G8" s="1"/>
+      <c r="H8" s="4"/>
+      <c r="AMJ8" s="0"/>
+    </row>
+    <row r="9" s="2" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1"/>
       <c r="C9" s="3"/>
       <c r="D9" s="27"/>
       <c r="E9" s="2" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="H9" s="1"/>
-      <c r="I9" s="4"/>
-    </row>
-    <row r="10" s="2" customFormat="true" ht="14.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>32</v>
+      </c>
+      <c r="G9" s="1"/>
+      <c r="H9" s="4"/>
+      <c r="AMJ9" s="0"/>
+    </row>
+    <row r="10" s="2" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1"/>
       <c r="C10" s="3"/>
       <c r="D10" s="27"/>
       <c r="E10" s="2" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="H10" s="1"/>
-      <c r="I10" s="4"/>
-    </row>
-    <row r="11" s="24" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>34</v>
+      </c>
+      <c r="G10" s="1"/>
+      <c r="H10" s="4"/>
+      <c r="AMJ10" s="0"/>
+    </row>
+    <row r="11" s="24" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="23"/>
       <c r="C11" s="25"/>
       <c r="D11" s="27"/>
       <c r="E11" s="24" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="F11" s="24" t="s">
-        <v>40</v>
-      </c>
-      <c r="H11" s="23"/>
-      <c r="I11" s="26"/>
-    </row>
-    <row r="12" s="31" customFormat="true" ht="14.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="1"/>
+        <v>36</v>
+      </c>
+      <c r="G11" s="23"/>
+      <c r="H11" s="26"/>
+      <c r="AMJ11" s="0"/>
+    </row>
+    <row r="12" s="31" customFormat="true" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="s">
+        <v>37</v>
+      </c>
       <c r="B12" s="28"/>
       <c r="C12" s="29"/>
-      <c r="D12" s="30"/>
-      <c r="H12" s="1"/>
-      <c r="I12" s="32"/>
+      <c r="D12" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="E12" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="F12" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="G12" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="H12" s="30"/>
+      <c r="I12" s="31" t="s">
+        <v>41</v>
+      </c>
+      <c r="AMJ12" s="0"/>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="32"/>
+      <c r="C13" s="33"/>
+      <c r="D13" s="18"/>
+      <c r="E13" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G13" s="34"/>
+      <c r="H13" s="35"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="D3:D4"/>
     <mergeCell ref="D5:D6"/>
     <mergeCell ref="D7:D11"/>
+    <mergeCell ref="D12:D13"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" display="Pi Pinout"/>
-    <hyperlink ref="I2" r:id="rId2" display="adafruit"/>
-    <hyperlink ref="I3" r:id="rId3" display="digikey"/>
+    <hyperlink ref="H2" r:id="rId2" display="adafruit"/>
+    <hyperlink ref="H3" r:id="rId3" display="digikey"/>
     <hyperlink ref="B7" r:id="rId4" display="adafruit"/>
-    <hyperlink ref="I7" r:id="rId5" display="digikey"/>
+    <hyperlink ref="H7" r:id="rId5" display="digikey"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>